<commit_message>
information package rename done better
</commit_message>
<xml_diff>
--- a/InformationPackageWorksheet.xlsx
+++ b/InformationPackageWorksheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\INFO3300_Learn_By_Doing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\GitHub\INFO3300_Learn_By_Doing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="28800" windowHeight="17055" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
@@ -617,23 +617,23 @@
       <selection activeCell="D4" sqref="D4:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -650,7 +650,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.8">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -664,7 +664,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.8">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -678,7 +678,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.8">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -692,7 +692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.8">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -706,7 +706,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -727,17 +727,17 @@
       <selection activeCell="A2" sqref="A2:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.95703125" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -748,7 +748,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -759,7 +759,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.8">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -782,7 +782,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.8">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -805,7 +805,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.8">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -828,7 +828,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.8">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
@@ -851,7 +851,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -872,7 +872,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.8">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -887,7 +887,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.8">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
New IP &&& lots of file structure changes... im ocd
</commit_message>
<xml_diff>
--- a/InformationPackageWorksheet.xlsx
+++ b/InformationPackageWorksheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="28800" windowHeight="17055" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="28800" windowHeight="17055" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>Information Subject: Clothing Shipments</t>
   </si>
@@ -99,53 +99,74 @@
     <t>Customer</t>
   </si>
   <si>
-    <t>Information Subject: ProductionBatch</t>
-  </si>
-  <si>
     <t xml:space="preserve">Compliance </t>
   </si>
   <si>
-    <t>OverallRating</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
-    <t>WorkerHealth</t>
-  </si>
-  <si>
-    <t>ConditionCategory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BaseCurrency </t>
-  </si>
-  <si>
     <t>Order</t>
   </si>
   <si>
-    <t>DeliveryNation</t>
-  </si>
-  <si>
-    <t>PriceAdjustment</t>
-  </si>
-  <si>
-    <t>OrderCurrency</t>
-  </si>
-  <si>
-    <t>OrderExchangeDate</t>
-  </si>
-  <si>
-    <t>Facts: QuantityProduced, QualityRating, EstEndTime, ActualEndTime, ProductionCost</t>
-  </si>
-  <si>
     <t>Gender</t>
+  </si>
+  <si>
+    <t>Information Subject: Production Batches</t>
+  </si>
+  <si>
+    <t>Condition Category</t>
+  </si>
+  <si>
+    <t>Overall Compliance Rating</t>
+  </si>
+  <si>
+    <t>Age Documents</t>
+  </si>
+  <si>
+    <t>Base Currency</t>
+  </si>
+  <si>
+    <t>Delivery Nation</t>
+  </si>
+  <si>
+    <t>Delivery State</t>
+  </si>
+  <si>
+    <t>Delivery City</t>
+  </si>
+  <si>
+    <t>Price Adjustment</t>
+  </si>
+  <si>
+    <t>Order Currency</t>
+  </si>
+  <si>
+    <t>Shipping Currency</t>
+  </si>
+  <si>
+    <t>Max Workers</t>
+  </si>
+  <si>
+    <t>List Price</t>
+  </si>
+  <si>
+    <t>Model Description</t>
+  </si>
+  <si>
+    <t>Base Price</t>
+  </si>
+  <si>
+    <t>Item Size</t>
+  </si>
+  <si>
+    <t>Facts: Quantity Produced, Quality Rating, Start Date, Estimated End Time, Actual End Time, ShipDate, Production Cost, Shipping Cost, Quantity Shipped,  Order Quantity, Order Sale Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -165,6 +186,21 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -261,28 +297,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -300,7 +347,6 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -334,15 +380,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:G9" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="1">
-  <tableColumns count="7">
-    <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2"/>
-    <tableColumn id="3" name="Column3"/>
-    <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Column5"/>
-    <tableColumn id="6" name="Column6"/>
-    <tableColumn id="7" name="Column7" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:F10" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="1">
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -610,7 +655,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
@@ -720,177 +765,166 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G10"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="1" max="1" width="10.625" style="4"/>
+    <col min="2" max="2" width="15.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.625" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="E7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="E8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="D9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
+      <c r="F9" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>